<commit_message>
Fix: working backend restored and ready for new features
</commit_message>
<xml_diff>
--- a/backend/projects.xlsx
+++ b/backend/projects.xlsx
@@ -460,22 +460,22 @@
         <v>239868</v>
       </c>
       <c r="G2" t="str">
-        <v>hgjb hbgvbgv  gggggg gggggggg gg</v>
+        <v xml:space="preserve">stud 1 stud 2 </v>
       </c>
       <c r="H2" t="str">
-        <v xml:space="preserve">ujuhyj vk hjuh vkjhyu nb     hjg vkg gjb yg yg yg hyb </v>
+        <v xml:space="preserve"> tergrthtty </v>
       </c>
       <c r="I2" t="str">
-        <v>1744006215277-bill.pdf</v>
+        <v>1744018445711-bill.pdf</v>
       </c>
       <c r="J2" t="str">
-        <v>1744006215280-bill.pdf</v>
+        <v>1744018445715-bill.pdf</v>
       </c>
       <c r="K2" t="str">
-        <v>someone@ssn.edu.in</v>
+        <v>bhuvana@ssn.edu.in</v>
       </c>
       <c r="L2" t="str">
-        <v>2025-04-07T06:10:15.289Z</v>
+        <v>2025-04-07T09:34:05.721Z</v>
       </c>
     </row>
   </sheetData>

</xml_diff>